<commit_message>
added battle data of all available dragons
</commit_message>
<xml_diff>
--- a/Dragons.xlsx
+++ b/Dragons.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="400">
   <si>
     <t>Name</t>
   </si>
@@ -1211,6 +1211,9 @@
   </si>
   <si>
     <t>Battle power</t>
+  </si>
+  <si>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -1553,8 +1556,8 @@
   <dimension ref="A1:H211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1616,6 +1619,9 @@
       <c r="G2" t="s">
         <v>30</v>
       </c>
+      <c r="H2">
+        <v>2397</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -1639,6 +1645,9 @@
       <c r="G3" t="s">
         <v>16</v>
       </c>
+      <c r="H3">
+        <v>4000</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
@@ -1662,6 +1671,9 @@
       <c r="G4" t="s">
         <v>16</v>
       </c>
+      <c r="H4">
+        <v>1058</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
@@ -1826,6 +1838,9 @@
       <c r="F11" t="s">
         <v>9</v>
       </c>
+      <c r="G11" t="s">
+        <v>399</v>
+      </c>
       <c r="H11">
         <v>1297</v>
       </c>
@@ -1872,6 +1887,9 @@
       <c r="F13" t="s">
         <v>9</v>
       </c>
+      <c r="G13" t="s">
+        <v>399</v>
+      </c>
       <c r="H13">
         <v>1772</v>
       </c>
@@ -2251,6 +2269,12 @@
       <c r="F30" t="s">
         <v>9</v>
       </c>
+      <c r="G30" t="s">
+        <v>399</v>
+      </c>
+      <c r="H30">
+        <v>2485</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
@@ -2294,6 +2318,9 @@
       <c r="F32" t="s">
         <v>9</v>
       </c>
+      <c r="G32" t="s">
+        <v>399</v>
+      </c>
       <c r="H32">
         <v>1238</v>
       </c>
@@ -2369,6 +2396,9 @@
       <c r="G35" t="s">
         <v>30</v>
       </c>
+      <c r="H35">
+        <v>2096</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
@@ -2392,6 +2422,9 @@
       <c r="G36" t="s">
         <v>16</v>
       </c>
+      <c r="H36">
+        <v>2440</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
@@ -2662,6 +2695,9 @@
       <c r="G48" t="s">
         <v>16</v>
       </c>
+      <c r="H48">
+        <v>1058</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
@@ -2780,6 +2816,9 @@
       <c r="G53" t="s">
         <v>16</v>
       </c>
+      <c r="H53">
+        <v>1058</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
@@ -2800,6 +2839,9 @@
       <c r="F54" t="s">
         <v>37</v>
       </c>
+      <c r="G54" t="s">
+        <v>399</v>
+      </c>
       <c r="H54">
         <v>1701</v>
       </c>
@@ -2826,6 +2868,9 @@
       <c r="G55" t="s">
         <v>30</v>
       </c>
+      <c r="H55">
+        <v>1195</v>
+      </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
@@ -2849,6 +2894,9 @@
       <c r="G56" t="s">
         <v>30</v>
       </c>
+      <c r="H56">
+        <v>1195</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
@@ -2872,6 +2920,9 @@
       <c r="G57" t="s">
         <v>16</v>
       </c>
+      <c r="H57">
+        <v>1326</v>
+      </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
@@ -2892,6 +2943,12 @@
       <c r="F58" t="s">
         <v>9</v>
       </c>
+      <c r="G58" t="s">
+        <v>399</v>
+      </c>
+      <c r="H58">
+        <v>1036</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
@@ -2915,6 +2972,9 @@
       <c r="G59" t="s">
         <v>16</v>
       </c>
+      <c r="H59">
+        <v>2262</v>
+      </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
@@ -3021,6 +3081,9 @@
       <c r="F64" t="s">
         <v>9</v>
       </c>
+      <c r="G64" t="s">
+        <v>399</v>
+      </c>
       <c r="H64">
         <v>1036</v>
       </c>
@@ -3133,6 +3196,9 @@
       <c r="F69" t="s">
         <v>179</v>
       </c>
+      <c r="G69" t="s">
+        <v>399</v>
+      </c>
       <c r="H69">
         <v>1036</v>
       </c>
@@ -3182,6 +3248,9 @@
       <c r="G71" t="s">
         <v>30</v>
       </c>
+      <c r="H71">
+        <v>2397</v>
+      </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
@@ -3274,6 +3343,9 @@
       <c r="G75" t="s">
         <v>30</v>
       </c>
+      <c r="H75">
+        <v>2798</v>
+      </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
@@ -3294,6 +3366,12 @@
       <c r="F76" t="s">
         <v>48</v>
       </c>
+      <c r="G76" t="s">
+        <v>399</v>
+      </c>
+      <c r="H76">
+        <v>2461</v>
+      </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
@@ -3314,6 +3392,12 @@
       <c r="F77" t="s">
         <v>9</v>
       </c>
+      <c r="G77" t="s">
+        <v>399</v>
+      </c>
+      <c r="H77">
+        <v>2366</v>
+      </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
@@ -3334,6 +3418,12 @@
       <c r="F78" t="s">
         <v>9</v>
       </c>
+      <c r="G78" t="s">
+        <v>399</v>
+      </c>
+      <c r="H78">
+        <v>1226</v>
+      </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
@@ -3357,6 +3447,9 @@
       <c r="G79" t="s">
         <v>30</v>
       </c>
+      <c r="H79">
+        <v>2076</v>
+      </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
@@ -3380,6 +3473,9 @@
       <c r="G80" t="s">
         <v>16</v>
       </c>
+      <c r="H80">
+        <v>2217</v>
+      </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
@@ -3403,6 +3499,9 @@
       <c r="G81" t="s">
         <v>30</v>
       </c>
+      <c r="H81">
+        <v>834</v>
+      </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
@@ -3423,6 +3522,12 @@
       <c r="F82" t="s">
         <v>9</v>
       </c>
+      <c r="G82" t="s">
+        <v>399</v>
+      </c>
+      <c r="H82">
+        <v>2271</v>
+      </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
@@ -3472,6 +3577,9 @@
       <c r="G84" t="s">
         <v>30</v>
       </c>
+      <c r="H84">
+        <v>1275</v>
+      </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
@@ -3492,6 +3600,12 @@
       <c r="F85" t="s">
         <v>9</v>
       </c>
+      <c r="G85" t="s">
+        <v>399</v>
+      </c>
+      <c r="H85">
+        <v>1084</v>
+      </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
@@ -3515,6 +3629,9 @@
       <c r="G86" t="s">
         <v>16</v>
       </c>
+      <c r="H86">
+        <v>1950</v>
+      </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
@@ -3538,6 +3655,9 @@
       <c r="G87" t="s">
         <v>30</v>
       </c>
+      <c r="H87">
+        <v>2798</v>
+      </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
@@ -3561,6 +3681,9 @@
       <c r="G88" t="s">
         <v>16</v>
       </c>
+      <c r="H88">
+        <v>1504</v>
+      </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
@@ -3581,6 +3704,12 @@
       <c r="F89" t="s">
         <v>9</v>
       </c>
+      <c r="G89" t="s">
+        <v>399</v>
+      </c>
+      <c r="H89">
+        <v>3031</v>
+      </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
@@ -3604,6 +3733,9 @@
       <c r="G90" t="s">
         <v>16</v>
       </c>
+      <c r="H90">
+        <v>924</v>
+      </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
@@ -3696,6 +3828,9 @@
       <c r="F94" t="s">
         <v>22</v>
       </c>
+      <c r="G94" t="s">
+        <v>399</v>
+      </c>
       <c r="H94">
         <v>1416</v>
       </c>
@@ -3851,6 +3986,12 @@
       <c r="F101" t="s">
         <v>9</v>
       </c>
+      <c r="G101" t="s">
+        <v>399</v>
+      </c>
+      <c r="H101">
+        <v>2366</v>
+      </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
@@ -3874,6 +4015,9 @@
       <c r="G102" t="s">
         <v>16</v>
       </c>
+      <c r="H102">
+        <v>2128</v>
+      </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
@@ -3995,6 +4139,9 @@
       <c r="F107" t="s">
         <v>15</v>
       </c>
+      <c r="G107" t="s">
+        <v>399</v>
+      </c>
       <c r="H107">
         <v>2889</v>
       </c>
@@ -4018,6 +4165,9 @@
       <c r="F108" t="s">
         <v>9</v>
       </c>
+      <c r="G108" t="s">
+        <v>399</v>
+      </c>
       <c r="H108">
         <v>1207</v>
       </c>
@@ -4041,6 +4191,12 @@
       <c r="F109" t="s">
         <v>9</v>
       </c>
+      <c r="G109" t="s">
+        <v>399</v>
+      </c>
+      <c r="H109">
+        <v>1036</v>
+      </c>
     </row>
     <row r="110" spans="1:8">
       <c r="A110" t="s">
@@ -4231,6 +4387,12 @@
       <c r="F117" t="s">
         <v>117</v>
       </c>
+      <c r="G117" t="s">
+        <v>399</v>
+      </c>
+      <c r="H117">
+        <v>3031</v>
+      </c>
     </row>
     <row r="118" spans="1:8">
       <c r="A118" t="s">
@@ -4251,6 +4413,9 @@
       <c r="F118" t="s">
         <v>9</v>
       </c>
+      <c r="G118" t="s">
+        <v>399</v>
+      </c>
       <c r="H118">
         <v>1131</v>
       </c>
@@ -4317,6 +4482,12 @@
       <c r="F121" t="s">
         <v>9</v>
       </c>
+      <c r="G121" t="s">
+        <v>399</v>
+      </c>
+      <c r="H121">
+        <v>1036</v>
+      </c>
     </row>
     <row r="122" spans="1:8">
       <c r="A122" t="s">
@@ -4337,6 +4508,12 @@
       <c r="F122" t="s">
         <v>129</v>
       </c>
+      <c r="G122" t="s">
+        <v>399</v>
+      </c>
+      <c r="H122">
+        <v>3696</v>
+      </c>
     </row>
     <row r="123" spans="1:8">
       <c r="A123" t="s">
@@ -4610,6 +4787,12 @@
       <c r="F134" t="s">
         <v>37</v>
       </c>
+      <c r="G134" t="s">
+        <v>399</v>
+      </c>
+      <c r="H134">
+        <v>2414</v>
+      </c>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" t="s">
@@ -4630,6 +4813,12 @@
       <c r="F135" t="s">
         <v>9</v>
       </c>
+      <c r="G135" t="s">
+        <v>399</v>
+      </c>
+      <c r="H135">
+        <v>1036</v>
+      </c>
     </row>
     <row r="136" spans="1:8">
       <c r="A136" t="s">
@@ -4653,6 +4842,9 @@
       <c r="G136" t="s">
         <v>16</v>
       </c>
+      <c r="H136">
+        <v>1593</v>
+      </c>
     </row>
     <row r="137" spans="1:8">
       <c r="A137" t="s">
@@ -4676,6 +4868,9 @@
       <c r="G137" t="s">
         <v>16</v>
       </c>
+      <c r="H137">
+        <v>1593</v>
+      </c>
     </row>
     <row r="138" spans="1:8">
       <c r="A138" t="s">
@@ -4696,6 +4891,12 @@
       <c r="F138" t="s">
         <v>15</v>
       </c>
+      <c r="G138" t="s">
+        <v>399</v>
+      </c>
+      <c r="H138">
+        <v>1701</v>
+      </c>
     </row>
     <row r="139" spans="1:8">
       <c r="A139" t="s">
@@ -4716,6 +4917,9 @@
       <c r="F139" t="s">
         <v>9</v>
       </c>
+      <c r="G139" t="s">
+        <v>399</v>
+      </c>
       <c r="H139">
         <v>1416</v>
       </c>
@@ -4762,6 +4966,9 @@
       <c r="G141" t="s">
         <v>30</v>
       </c>
+      <c r="H141">
+        <v>2036</v>
+      </c>
     </row>
     <row r="142" spans="1:8">
       <c r="A142" t="s">
@@ -4785,6 +4992,9 @@
       <c r="G142" t="s">
         <v>16</v>
       </c>
+      <c r="H142">
+        <v>2217</v>
+      </c>
     </row>
     <row r="143" spans="1:8">
       <c r="A143" t="s">
@@ -4805,6 +5015,12 @@
       <c r="F143" t="s">
         <v>351</v>
       </c>
+      <c r="G143" t="s">
+        <v>399</v>
+      </c>
+      <c r="H143">
+        <v>3506</v>
+      </c>
     </row>
     <row r="144" spans="1:8">
       <c r="A144" t="s">
@@ -4897,6 +5113,9 @@
       <c r="F147" t="s">
         <v>22</v>
       </c>
+      <c r="G147" t="s">
+        <v>399</v>
+      </c>
       <c r="H147">
         <v>1891</v>
       </c>
@@ -4969,6 +5188,9 @@
       <c r="F150" t="s">
         <v>22</v>
       </c>
+      <c r="G150" t="s">
+        <v>399</v>
+      </c>
       <c r="H150">
         <v>1654</v>
       </c>
@@ -5018,6 +5240,12 @@
       <c r="F152" t="s">
         <v>37</v>
       </c>
+      <c r="G152" t="s">
+        <v>399</v>
+      </c>
+      <c r="H152">
+        <v>3934</v>
+      </c>
     </row>
     <row r="153" spans="1:8">
       <c r="A153" t="s">
@@ -5041,6 +5269,9 @@
       <c r="G153" t="s">
         <v>16</v>
       </c>
+      <c r="H153">
+        <v>1620</v>
+      </c>
     </row>
     <row r="154" spans="1:8">
       <c r="A154" t="s">
@@ -5064,6 +5295,9 @@
       <c r="G154" t="s">
         <v>16</v>
       </c>
+      <c r="H154">
+        <v>1620</v>
+      </c>
     </row>
     <row r="155" spans="1:8">
       <c r="A155" t="s">
@@ -5084,6 +5318,12 @@
       <c r="F155" t="s">
         <v>9</v>
       </c>
+      <c r="G155" t="s">
+        <v>399</v>
+      </c>
+      <c r="H155">
+        <v>1036</v>
+      </c>
     </row>
     <row r="156" spans="1:8">
       <c r="A156" t="s">
@@ -5104,6 +5344,12 @@
       <c r="F156" t="s">
         <v>9</v>
       </c>
+      <c r="G156" t="s">
+        <v>399</v>
+      </c>
+      <c r="H156">
+        <v>2271</v>
+      </c>
     </row>
     <row r="157" spans="1:8">
       <c r="A157" t="s">
@@ -5150,6 +5396,12 @@
       <c r="F158" t="s">
         <v>15</v>
       </c>
+      <c r="G158" t="s">
+        <v>399</v>
+      </c>
+      <c r="H158">
+        <v>2414</v>
+      </c>
     </row>
     <row r="159" spans="1:8">
       <c r="A159" t="s">
@@ -5170,8 +5422,11 @@
       <c r="F159" t="s">
         <v>20</v>
       </c>
+      <c r="G159" t="s">
+        <v>399</v>
+      </c>
       <c r="H159">
-        <v>2485</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5196,6 +5451,9 @@
       <c r="G160" t="s">
         <v>16</v>
       </c>
+      <c r="H160">
+        <v>2387</v>
+      </c>
     </row>
     <row r="161" spans="1:8">
       <c r="A161" t="s">
@@ -5268,6 +5526,9 @@
       <c r="G163" t="s">
         <v>30</v>
       </c>
+      <c r="H163">
+        <v>2197</v>
+      </c>
     </row>
     <row r="164" spans="1:8">
       <c r="A164" t="s">
@@ -5308,6 +5569,9 @@
       <c r="F165" t="s">
         <v>22</v>
       </c>
+      <c r="G165" t="s">
+        <v>399</v>
+      </c>
       <c r="H165">
         <v>989</v>
       </c>
@@ -5406,6 +5670,12 @@
       <c r="F169" t="s">
         <v>9</v>
       </c>
+      <c r="G169" t="s">
+        <v>399</v>
+      </c>
+      <c r="H169">
+        <v>1036</v>
+      </c>
     </row>
     <row r="170" spans="1:8">
       <c r="A170" t="s">
@@ -5455,6 +5725,9 @@
       <c r="G171" t="s">
         <v>30</v>
       </c>
+      <c r="H171">
+        <v>2036</v>
+      </c>
     </row>
     <row r="172" spans="1:8">
       <c r="A172" t="s">
@@ -5498,6 +5771,9 @@
       <c r="G173" t="s">
         <v>16</v>
       </c>
+      <c r="H173">
+        <v>2262</v>
+      </c>
     </row>
     <row r="174" spans="1:8">
       <c r="A174" t="s">
@@ -5567,6 +5843,9 @@
       <c r="G176" t="s">
         <v>16</v>
       </c>
+      <c r="H176">
+        <v>2841</v>
+      </c>
     </row>
     <row r="177" spans="1:8">
       <c r="A177" t="s">
@@ -5636,6 +5915,9 @@
       <c r="F179" t="s">
         <v>9</v>
       </c>
+      <c r="G179" t="s">
+        <v>399</v>
+      </c>
       <c r="H179">
         <v>1226</v>
       </c>
@@ -5725,6 +6007,9 @@
       <c r="F183" t="s">
         <v>11</v>
       </c>
+      <c r="G183" t="s">
+        <v>399</v>
+      </c>
       <c r="H183">
         <v>3079</v>
       </c>
@@ -5774,6 +6059,9 @@
       <c r="F185" t="s">
         <v>9</v>
       </c>
+      <c r="G185" t="s">
+        <v>399</v>
+      </c>
       <c r="H185">
         <v>894</v>
       </c>
@@ -5820,6 +6108,9 @@
       <c r="F187" t="s">
         <v>22</v>
       </c>
+      <c r="G187" t="s">
+        <v>399</v>
+      </c>
       <c r="H187">
         <v>1796</v>
       </c>
@@ -5843,6 +6134,12 @@
       <c r="F188" t="s">
         <v>9</v>
       </c>
+      <c r="G188" t="s">
+        <v>399</v>
+      </c>
+      <c r="H188">
+        <v>3506</v>
+      </c>
     </row>
     <row r="189" spans="1:8">
       <c r="A189" t="s">
@@ -5886,6 +6183,9 @@
       <c r="G190" t="s">
         <v>16</v>
       </c>
+      <c r="H190">
+        <v>2663</v>
+      </c>
     </row>
     <row r="191" spans="1:8">
       <c r="A191" t="s">
@@ -5958,6 +6258,12 @@
       <c r="F193" t="s">
         <v>20</v>
       </c>
+      <c r="G193" t="s">
+        <v>399</v>
+      </c>
+      <c r="H193">
+        <v>2414</v>
+      </c>
     </row>
     <row r="194" spans="1:8">
       <c r="A194" t="s">
@@ -6168,6 +6474,9 @@
       <c r="G202" t="s">
         <v>16</v>
       </c>
+      <c r="H202">
+        <v>2958</v>
+      </c>
     </row>
     <row r="203" spans="1:8">
       <c r="A203" t="s">
@@ -6335,6 +6644,9 @@
       <c r="G209" t="s">
         <v>30</v>
       </c>
+      <c r="H209">
+        <v>2397</v>
+      </c>
     </row>
     <row r="210" spans="1:8">
       <c r="A210" t="s">
@@ -6377,6 +6689,9 @@
       </c>
       <c r="F211" t="s">
         <v>20</v>
+      </c>
+      <c r="G211" t="s">
+        <v>399</v>
       </c>
       <c r="H211">
         <v>2366</v>

</xml_diff>